<commit_message>
add loess, change fig1
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B6ABBB-6386-4980-8537-F2E92E60D30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10947D8-8BA6-4AE9-8364-B87F37088D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,11 +419,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>72.5</v>
+        <v>73</v>
       </c>
       <c r="F2" s="3">
         <f>50*D2</f>
-        <v>3625</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -537,6 +537,14 @@
       </c>
       <c r="B16">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45111</v>
+      </c>
+      <c r="B17">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simplify with new functions
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDA01B1-6FB7-4273-B790-49C61089D338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9B7B6B-15AD-4810-A770-63293C8A1B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,7 +385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
@@ -419,11 +419,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>81</v>
+        <v>87.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>3240</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -585,6 +585,14 @@
       </c>
       <c r="B22">
         <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45172</v>
+      </c>
+      <c r="B23">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add remaining functions from
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602E62B0-CF21-4B5F-BB6F-A17607C6086E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871BB8BC-0F7F-4C6F-B145-6462E53882BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,11 +419,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>3600</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -601,6 +601,14 @@
       </c>
       <c r="B24">
         <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45179</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
science + nature data
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA824922-2029-4AC6-B167-3FBCB604693F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6970AB81-5A54-4EEC-ABFD-7ACEF38560EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,11 +419,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>4200</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -625,6 +625,30 @@
       </c>
       <c r="B27">
         <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45191</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45192</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45193</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
closes #6, closes #7, closes #8, + work on landing page
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECB95E7-55B2-4F49-B630-E2E8F69EB793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B537CF6E-F9D8-4619-83AA-70D85455D3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,16 +94,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -385,19 +396,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -409,7 +420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45073</v>
       </c>
@@ -417,72 +428,104 @@
         <f>1+2+4</f>
         <v>7</v>
       </c>
+      <c r="C2">
+        <f>B2</f>
+        <v>7</v>
+      </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>116</v>
+        <v>118.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>4640</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4740</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45074</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f>C2+B3</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45076</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f t="shared" ref="C4:C33" si="0">C3+B4</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45080</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45081</v>
       </c>
       <c r="B6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45082</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45085</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45086</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45087</v>
       </c>
@@ -490,181 +533,286 @@
         <f>3.5</f>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45088</v>
       </c>
       <c r="B11">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45094</v>
       </c>
       <c r="B12">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>53.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>45095</v>
       </c>
       <c r="B13">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>45096</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45102</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45103</v>
       </c>
       <c r="B16">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>45111</v>
       </c>
       <c r="B17">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>45112</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>45114</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>45115</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>45123</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>45124</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45172</v>
       </c>
       <c r="B23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45178</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
         <v>45179</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="5">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>45185</v>
       </c>
       <c r="B26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>45186</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45191</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45192</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45193</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45199</v>
       </c>
       <c r="B31">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>113.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45200</v>
       </c>
       <c r="B32">
         <v>2.5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>45336</v>
+      </c>
+      <c r="B33">
+        <v>2.5</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>118.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweak Project landing page and methods section, rest still needs to be adjusted
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B537CF6E-F9D8-4619-83AA-70D85455D3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11C7D70-2AFE-4811-BFD7-66CBB3D4705F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>118.5</v>
+        <v>120</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>4740</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -808,11 +808,11 @@
         <v>45336</v>
       </c>
       <c r="B33">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>118.5</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update about the authors
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BD197A-E82C-4F60-A75E-05ED5A48A131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5F8103-FFBD-40AA-BBBB-62CD695E7D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>121</v>
+        <v>121.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>4840</v>
+        <v>4860</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -825,6 +825,18 @@
       <c r="C34">
         <f t="shared" ref="C34" si="1">C33+B34</f>
         <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>45345</v>
+      </c>
+      <c r="B35">
+        <v>0.5</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35" si="2">C34+B35</f>
+        <v>121.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bringing corrections to journals
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D008D32E-F477-4BE6-A8EC-E158FE8B54D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D74572A-8931-4E03-A111-88EC8D1E6517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>128</v>
+        <v>130.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>5120</v>
+        <v>5220</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -909,6 +909,18 @@
       <c r="C41">
         <f t="shared" si="5"/>
         <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>45360</v>
+      </c>
+      <c r="B42">
+        <v>2.5</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ref="C42" si="6">C41+B42</f>
+        <v>130.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
closes #14 and closes #1
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECD94F0-D78A-45EE-B188-B2E9D4284040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CD0527-3F0A-4532-8875-D799EA96A65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>140.5</v>
+        <v>144</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>5620</v>
+        <v>5760</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -993,6 +993,18 @@
       <c r="C48">
         <f t="shared" si="9"/>
         <v>140.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>45393</v>
+      </c>
+      <c r="B49">
+        <v>3.5</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49" si="10">C48+B49</f>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix #42 and fix 44
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CD0527-3F0A-4532-8875-D799EA96A65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29F7234-AA57-47D4-8D9E-4D7BE8E9BA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>144</v>
+        <v>146.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>5760</v>
+        <v>5860</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1003,8 +1003,32 @@
         <v>3.5</v>
       </c>
       <c r="C49">
-        <f t="shared" ref="C49" si="10">C48+B49</f>
+        <f t="shared" ref="C49:C50" si="10">C48+B49</f>
         <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>45401</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="10"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>45403</v>
+      </c>
+      <c r="B51">
+        <v>1.5</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51" si="11">C50+B51</f>
+        <v>146.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
attempts to add citation #43
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29F7234-AA57-47D4-8D9E-4D7BE8E9BA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B96E6E3-F411-4CDC-969F-E77A74CB8F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>146.5</v>
+        <v>147</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>5860</v>
+        <v>5880</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1024,11 +1024,11 @@
         <v>45403</v>
       </c>
       <c r="B51">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C51">
         <f t="shared" ref="C51" si="11">C50+B51</f>
-        <v>146.5</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separate fields into children scripts
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663503D4-0F81-4918-9DAB-079390847E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF839886-1E48-4508-B98A-1DF12627C347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>147.5</v>
+        <v>149.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>5900</v>
+        <v>5980</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1041,6 +1041,18 @@
       <c r="C52">
         <f t="shared" ref="C52" si="12">C51+B52</f>
         <v>147.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>45410</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ref="C53" si="13">C52+B53</f>
+        <v>149.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing different plot layouts for #35
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19215085-1748-462E-8973-AEA47356DD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9C8058-A1A2-4E54-83D2-09D2493D933F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>153.5</v>
+        <v>155</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>6140</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1063,7 +1063,7 @@
         <v>2.5</v>
       </c>
       <c r="C54">
-        <f t="shared" ref="C54:C55" si="14">C53+B54</f>
+        <f t="shared" ref="C54:C57" si="14">C53+B54</f>
         <v>152</v>
       </c>
     </row>
@@ -1077,6 +1077,30 @@
       <c r="C55">
         <f t="shared" si="14"/>
         <v>153.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>45419</v>
+      </c>
+      <c r="B56">
+        <v>0.5</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="14"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>45421</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="14"/>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move to new package pubDashboard and openAlex, delete old data, closes #35
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9C8058-A1A2-4E54-83D2-09D2493D933F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAF05E8-F9D8-41E4-8E75-4D4DDC3A32CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>6200</v>
+        <v>6800</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1096,11 +1096,71 @@
         <v>45421</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C57">
         <f t="shared" si="14"/>
-        <v>155</v>
+        <v>155.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>45424</v>
+      </c>
+      <c r="B58">
+        <v>6</v>
+      </c>
+      <c r="C58">
+        <f>C57+B58</f>
+        <v>161.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>45426</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <f t="shared" ref="C59" si="15">C58+B59</f>
+        <v>163.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>45427</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <f t="shared" ref="C60" si="16">C59+B60</f>
+        <v>165.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>45428</v>
+      </c>
+      <c r="B61">
+        <v>2.5</v>
+      </c>
+      <c r="C61">
+        <f t="shared" ref="C61:C62" si="17">C60+B61</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>45429</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="17"/>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all new openalex data, closes #40, closes #38, closes #37, closes #39
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAF05E8-F9D8-41E4-8E75-4D4DDC3A32CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD55630E-6E00-4FB6-BE88-1CD74DB02211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>170</v>
+        <v>177.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>6800</v>
+        <v>7100</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1156,11 +1156,23 @@
         <v>45429</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="C62">
         <f t="shared" si="17"/>
-        <v>170</v>
+        <v>170.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>45430</v>
+      </c>
+      <c r="B63">
+        <v>7</v>
+      </c>
+      <c r="C63">
+        <f t="shared" ref="C63" si="18">C62+B63</f>
+        <v>177.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust configurations, closes #46
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD55630E-6E00-4FB6-BE88-1CD74DB02211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3227B1E-D3B2-4F50-BAC9-074F819F7708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>177.5</v>
+        <v>179</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>7100</v>
+        <v>7160</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1168,11 +1168,11 @@
         <v>45430</v>
       </c>
       <c r="B63">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="C63">
         <f t="shared" ref="C63" si="18">C62+B63</f>
-        <v>177.5</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove general journals from landing page gauges
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3227B1E-D3B2-4F50-BAC9-074F819F7708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3743CA1B-AF85-42DD-A2A9-B4D92AE03B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>179</v>
+        <v>184.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>7160</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1171,8 +1171,20 @@
         <v>8.5</v>
       </c>
       <c r="C63">
-        <f t="shared" ref="C63" si="18">C62+B63</f>
+        <f t="shared" ref="C63:C64" si="18">C62+B63</f>
         <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>45432</v>
+      </c>
+      <c r="B64">
+        <v>5.5</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="18"/>
+        <v>184.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust navigation and add clarity on data
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3743CA1B-AF85-42DD-A2A9-B4D92AE03B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8F7F09-0B7A-4D08-B3BC-4C323B3CFEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>184.5</v>
+        <v>185.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>7380</v>
+        <v>7420</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1180,11 +1180,11 @@
         <v>45432</v>
       </c>
       <c r="B64">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="C64">
         <f t="shared" si="18"/>
-        <v>184.5</v>
+        <v>185.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change header menu, change figure instructions to reusable object for consistency, change scatter_country_year to loess instead of lm
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8F7F09-0B7A-4D08-B3BC-4C323B3CFEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3B741B-2F18-4855-8FAB-C1EB39CCAE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>185.5</v>
+        <v>187</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>7420</v>
+        <v>7480</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1180,11 +1180,11 @@
         <v>45432</v>
       </c>
       <c r="B64">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="C64">
         <f t="shared" si="18"/>
-        <v>185.5</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shorten instructions, change navmenu
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3B741B-2F18-4855-8FAB-C1EB39CCAE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E53974-2733-41F6-8EC3-119DC7C641DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>7480</v>
+        <v>7560</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1171,7 +1171,7 @@
         <v>8.5</v>
       </c>
       <c r="C63">
-        <f t="shared" ref="C63:C64" si="18">C62+B63</f>
+        <f t="shared" ref="C63:C66" si="18">C62+B63</f>
         <v>179</v>
       </c>
     </row>
@@ -1185,6 +1185,30 @@
       <c r="C64">
         <f t="shared" si="18"/>
         <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>45433</v>
+      </c>
+      <c r="B65">
+        <v>1.5</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="18"/>
+        <v>188.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>45434</v>
+      </c>
+      <c r="B66">
+        <v>0.5</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="18"/>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor updates after changes to package
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9B244E-2ABB-456F-B0C7-2FC55D55C807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566AAC63-C674-4364-B461-39ABF4418045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>191</v>
+        <v>194.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>7640</v>
+        <v>7780</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1221,6 +1221,18 @@
       <c r="C67">
         <f t="shared" si="18"/>
         <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>45443</v>
+      </c>
+      <c r="B68">
+        <v>3.5</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ref="C68" si="19">C67+B68</f>
+        <v>194.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
attempt to add journal by year
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\forks\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566AAC63-C674-4364-B461-39ABF4418045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BEFB3E-BCFA-4417-9C02-76A426164EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,19 +396,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -420,7 +420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45073</v>
       </c>
@@ -434,14 +434,14 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>194.5</v>
+        <v>206.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>7780</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45074</v>
       </c>
@@ -453,7 +453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45076</v>
       </c>
@@ -465,7 +465,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45080</v>
       </c>
@@ -477,7 +477,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45081</v>
       </c>
@@ -489,7 +489,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45082</v>
       </c>
@@ -501,7 +501,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45085</v>
       </c>
@@ -513,7 +513,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45086</v>
       </c>
@@ -525,7 +525,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45087</v>
       </c>
@@ -538,7 +538,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45088</v>
       </c>
@@ -550,7 +550,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45094</v>
       </c>
@@ -562,7 +562,7 @@
         <v>53.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45095</v>
       </c>
@@ -574,7 +574,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45096</v>
       </c>
@@ -586,7 +586,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45102</v>
       </c>
@@ -598,7 +598,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45103</v>
       </c>
@@ -610,7 +610,7 @@
         <v>72.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45111</v>
       </c>
@@ -622,7 +622,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45112</v>
       </c>
@@ -634,7 +634,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45114</v>
       </c>
@@ -646,7 +646,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45115</v>
       </c>
@@ -658,7 +658,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45123</v>
       </c>
@@ -670,7 +670,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45124</v>
       </c>
@@ -682,7 +682,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45172</v>
       </c>
@@ -694,7 +694,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45178</v>
       </c>
@@ -706,7 +706,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>45179</v>
       </c>
@@ -719,7 +719,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45185</v>
       </c>
@@ -731,7 +731,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45186</v>
       </c>
@@ -743,7 +743,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45191</v>
       </c>
@@ -755,7 +755,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45192</v>
       </c>
@@ -767,7 +767,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45193</v>
       </c>
@@ -779,7 +779,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45199</v>
       </c>
@@ -791,7 +791,7 @@
         <v>113.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45200</v>
       </c>
@@ -803,7 +803,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45336</v>
       </c>
@@ -815,7 +815,7 @@
         <v>120.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45344</v>
       </c>
@@ -827,7 +827,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45345</v>
       </c>
@@ -839,7 +839,7 @@
         <v>121.5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45346</v>
       </c>
@@ -851,7 +851,7 @@
         <v>122.5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45347</v>
       </c>
@@ -863,7 +863,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45354</v>
       </c>
@@ -875,7 +875,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45356</v>
       </c>
@@ -887,7 +887,7 @@
         <v>125.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45358</v>
       </c>
@@ -899,7 +899,7 @@
         <v>126.5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45359</v>
       </c>
@@ -911,7 +911,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45360</v>
       </c>
@@ -923,7 +923,7 @@
         <v>130.5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45361</v>
       </c>
@@ -935,7 +935,7 @@
         <v>134.5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45363</v>
       </c>
@@ -947,7 +947,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45364</v>
       </c>
@@ -959,7 +959,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45366</v>
       </c>
@@ -971,7 +971,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45367</v>
       </c>
@@ -983,7 +983,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45368</v>
       </c>
@@ -995,7 +995,7 @@
         <v>140.5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45393</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45401</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45403</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45408</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>147.5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45410</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>149.5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45411</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45412</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>153.5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45419</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45421</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>155.5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45424</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>161.5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45426</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>163.5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45427</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>165.5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45428</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45429</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>170.5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45430</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45432</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45433</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>188.5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45434</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45442</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45443</v>
       </c>
@@ -1231,8 +1231,45 @@
         <v>3.5</v>
       </c>
       <c r="C68">
-        <f t="shared" ref="C68" si="19">C67+B68</f>
+        <f t="shared" ref="C68:C69" si="19">C67+B68</f>
         <v>194.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>45537</v>
+      </c>
+      <c r="B69" s="5">
+        <f>3+3</f>
+        <v>6</v>
+      </c>
+      <c r="C69" s="5">
+        <f t="shared" si="19"/>
+        <v>200.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>45541</v>
+      </c>
+      <c r="B70">
+        <v>3</v>
+      </c>
+      <c r="C70">
+        <f t="shared" ref="C70" si="20">C69+B70</f>
+        <v>203.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>45542</v>
+      </c>
+      <c r="B71">
+        <v>3</v>
+      </c>
+      <c r="C71">
+        <f t="shared" ref="C71" si="21">C70+B71</f>
+        <v>206.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add experimental shiny journal selector...
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\forks\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012BD772-2B20-4A01-981A-BC6F1CD6F833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182F16BE-B5DA-40E5-B6EE-572B671279EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>213</v>
+        <v>215.5</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>8520</v>
+        <v>8620</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1268,7 +1268,7 @@
         <v>3</v>
       </c>
       <c r="C71">
-        <f t="shared" ref="C71:C72" si="21">C70+B71</f>
+        <f t="shared" ref="C71:C73" si="21">C70+B71</f>
         <v>206.5</v>
       </c>
     </row>
@@ -1282,6 +1282,18 @@
       <c r="C72">
         <f t="shared" si="21"/>
         <v>213</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>45544</v>
+      </c>
+      <c r="B73">
+        <v>2.5</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="21"/>
+        <v>215.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove experimental shiny tab...
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\forks\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182F16BE-B5DA-40E5-B6EE-572B671279EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA70D8B-CF75-46E7-B418-EB13D5769927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>215.5</v>
+        <v>218</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>8620</v>
+        <v>8720</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1289,11 +1289,11 @@
         <v>45544</v>
       </c>
       <c r="B73">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="C73">
         <f t="shared" si="21"/>
-        <v>215.5</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
readd data shiny, add methods and missing data sections
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\forks\busara_dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA70D8B-CF75-46E7-B418-EB13D5769927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B3AD47-B996-4EED-AD4C-ED8B5D1A69DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>8720</v>
+        <v>9440</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1268,7 +1268,7 @@
         <v>3</v>
       </c>
       <c r="C71">
-        <f t="shared" ref="C71:C73" si="21">C70+B71</f>
+        <f t="shared" ref="C71:C76" si="21">C70+B71</f>
         <v>206.5</v>
       </c>
     </row>
@@ -1294,6 +1294,42 @@
       <c r="C73">
         <f t="shared" si="21"/>
         <v>218</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>45629</v>
+      </c>
+      <c r="B74">
+        <v>8</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="21"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>45643</v>
+      </c>
+      <c r="B75">
+        <v>7</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="21"/>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>45644</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="21"/>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
consistency for header names
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B3AD47-B996-4EED-AD4C-ED8B5D1A69DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A385E481-7876-4B78-95A7-5C18061BC1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>9440</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1330,6 +1330,30 @@
       <c r="C76">
         <f t="shared" si="21"/>
         <v>236</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>45645</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <f t="shared" ref="C77" si="22">C76+B77</f>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>45646</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="C78">
+        <f t="shared" ref="C78" si="23">C77+B78</f>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include shiny for gauges and correct journal menu bug (global sidebar)
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\busara_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A385E481-7876-4B78-95A7-5C18061BC1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3989B566-FFC0-4228-9E56-16F7EF887755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,11 +434,11 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F2" s="3">
         <f>40*D2</f>
-        <v>9600</v>
+        <v>9640</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,8 +1352,20 @@
         <v>3</v>
       </c>
       <c r="C78">
-        <f t="shared" ref="C78" si="23">C77+B78</f>
+        <f t="shared" ref="C78:C79" si="23">C77+B78</f>
         <v>240</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>45649</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="23"/>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>